<commit_message>
feat: added excel limit function for sentiment output
</commit_message>
<xml_diff>
--- a/model_input.xlsx
+++ b/model_input.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -37,7 +37,7 @@
 So if you like driving enthusiastically then this might be another factor to consider.</t>
   </si>
   <si>
-    <t>[deleted]</t>
+    <t>Most likely I will go in for automatic Petrol car for now. CNG means it would run first on petrol then switch to CNG. If you are running you can only on CNG, its gonna get fucked. I am not sure abt LPG. CNG stations are there in north goa and you don't need to fill in the gas like every other day. Once a month should be fine.</t>
   </si>
   <si>
     <t>For now I will stick to Automatic cars. As and when CNG becomes a viable alternative I will consider that. I am planning on Suzuki/Maruti so quite positive they might fit the CNG later. I might not even go for CNG if the engine and other problems are way too much. 
@@ -84,14 +84,15 @@
 which automatic is more compatible with CNG, CVT/IMT/AMT etc.</t>
   </si>
   <si>
-    <t>Most likely I will go in for automatic Petrol car for now. CNG means it would run first on petrol then switch to CNG. If you are running you can only on CNG, its gonna get fucked. I am not sure abt LPG. CNG stations are there in north goa and you don't need to fill in the gas like every other day. Once a month should be fine.</t>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,10 +103,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,16 +126,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -143,17 +143,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -162,10 +176,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -203,69 +217,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -289,54 +305,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -346,7 +361,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -355,7 +370,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -364,7 +379,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -372,10 +387,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -404,7 +419,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -417,13 +432,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -441,115 +455,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="140.71928571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="32.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="45.75">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="45.75">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="45.75">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="84.75">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: fix and remove some files
</commit_message>
<xml_diff>
--- a/model_input.xlsx
+++ b/model_input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="1443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="1438">
   <si>
     <t>comments</t>
   </si>
@@ -4313,12 +4313,6 @@
     <t>Because they want more space? Because maybe they have a bigger family? Maybe because they want to and its their own money? Not everyone buys a suv to go off road</t>
   </si>
   <si>
-    <t>I posted this from Guru Gram</t>
-  </si>
-  <si>
-    <t>I totally do, bro</t>
-  </si>
-  <si>
     <t>But they clearly can no? To afford to install an ~60-70k cng kit, to drive the car wherever they want without any major drawbacks with less carbon emissions too. I don't see how he's losing on this one</t>
   </si>
   <si>
@@ -4351,9 +4345,6 @@
   </si>
   <si>
     <t>Yeah 10 years back  I saw accords and civics running on cng here back in delhi</t>
-  </si>
-  <si>
-    <t>Just why</t>
   </si>
   <si>
     <t>Goli bhai itni average nahi aati. Agar aati hoti to sab log cng hi chala rahe hote, literally aadha price lol.</t>
@@ -4471,12 +4462,6 @@
 CNG kits have auto shut-off valves in case of impact, and the tanks are much thicker than petrol tanks. The force needed to damage a CNG tank would destroy the entire rear end of the car, including a petrol tank. Technically it's petrol tanks that are unsafe when compared.
 And about the filling process? CNG stations REFUSE to fill a car if it hasn’t passed tank testing. There's a plate near the valve with the date on it, and the tank has to be tested every 3-5 years. Petrol tanks never get tested post purchase even after having a higher flammability. So you tell me, you're driving a petrol car around, is that worth more than a human life?
 Wouldn't be surprised if the answer would be a resounding YES!</t>
-  </si>
-  <si>
-    <t>70k</t>
-  </si>
-  <si>
-    <t>Naah mate. Bangalore is a hell hole that I left behind a long time back.</t>
   </si>
   <si>
     <t>No way bro💀💀</t>
@@ -4879,7 +4864,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A1604"/>
+  <dimension ref="A1:A1599"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -12881,31 +12866,6 @@
         <v>1437</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="1600" customHeight="1" ht="18.75">
-      <c r="A1600" s="2" t="s">
-        <v>1438</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="1601" customHeight="1" ht="18.75">
-      <c r="A1601" s="2" t="s">
-        <v>1439</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="1602" customHeight="1" ht="18.75">
-      <c r="A1602" s="2" t="s">
-        <v>1440</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="1603" customHeight="1" ht="18.75">
-      <c r="A1603" s="2" t="s">
-        <v>1441</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="1604" customHeight="1" ht="18.75">
-      <c r="A1604" s="2" t="s">
-        <v>1442</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>